<commit_message>
Working test influxDB writter to test the online state Update DB mapping to include the docker compose containers docker-compose to create grafana and influxDB
</commit_message>
<xml_diff>
--- a/backend/v1.0/mockDB/Registros_Modbus.xlsx
+++ b/backend/v1.0/mockDB/Registros_Modbus.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SMARTGRID_CALI\backend\v1.0\mockDB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EUSSE\Desktop\proyecto-cali-backend\backend\v1.0\mockDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60BE1B8-6C49-4162-9858-636AD635ECEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C279000-AACE-4E6A-A32B-49F403B87E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ConexionDB" sheetId="4" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="466">
   <si>
     <t xml:space="preserve">0x0002 </t>
   </si>
@@ -1469,6 +1469,9 @@
   </si>
   <si>
     <t>4pJB_298afu0WKjKBtPESjnUxvpJV0PODWBNMGzeeU_ahg1P4H3Bg5KOfwI2A9LXm2BQwaQR_un792HXy3bsvg==</t>
+  </si>
+  <si>
+    <t>Laboratorio0. Token</t>
   </si>
 </sst>
 </file>
@@ -1839,7 +1842,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1908,11 +1911,32 @@
         <v>464</v>
       </c>
     </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>436</v>
+      </c>
+      <c r="B4" t="s">
+        <v>437</v>
+      </c>
+      <c r="C4">
+        <v>8086</v>
+      </c>
+      <c r="D4" t="s">
+        <v>440</v>
+      </c>
+      <c r="E4" t="s">
+        <v>438</v>
+      </c>
+      <c r="F4" t="s">
+        <v>465</v>
+      </c>
+    </row>
     <row r="10" spans="1:6">
       <c r="E10" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Change in DB names and requirements.txt
</commit_message>
<xml_diff>
--- a/backend/v1.0/mockDB/Registros_Modbus.xlsx
+++ b/backend/v1.0/mockDB/Registros_Modbus.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Betan\Documents\GitHub\project-cali\backend\v1.0\mockDB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EUSSE\Desktop\proyecto-cali-backend\backend\v1.0\mockDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24F4F13-B3A8-43CA-8F32-B69876196D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D91023-A9FC-4C10-B645-5D902403F50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ConexionDB" sheetId="4" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="469">
   <si>
     <t xml:space="preserve">0x0002 </t>
   </si>
@@ -1478,6 +1478,9 @@
   </si>
   <si>
     <t>Laboratorio_Energías</t>
+  </si>
+  <si>
+    <t>Laboratorio</t>
   </si>
 </sst>
 </file>
@@ -1849,7 +1852,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1930,7 +1933,7 @@
         <v>8086</v>
       </c>
       <c r="D4" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="E4" t="s">
         <v>438</v>

</xml_diff>